<commit_message>
Update E Commerce Project spreadsheet with latest data
</commit_message>
<xml_diff>
--- a/01_BaseLine/BL01/E Commerce Project.xlsx
+++ b/01_BaseLine/BL01/E Commerce Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoang\E_Commerce_Test\01_BaseLine\BL01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C7DAD1-E510-4EFA-B3CA-6249F4EB1B42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E06ECE-660C-4D2A-B339-9D2D8FDCFFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Login" sheetId="3" r:id="rId3"/>
     <sheet name="Register" sheetId="4" r:id="rId4"/>
     <sheet name="Logout" sheetId="5" r:id="rId5"/>
+    <sheet name="Forgot Password" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="410">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1417,6 +1418,134 @@
   </si>
   <si>
     <t>Validate the working of Logout functionality</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Forgotten Password' page
+2. Success message with text - 'An email with a confirmation link has been sent your email address.' should be displayed in green color
+3. Validate that an email is received regarding resseting of the password to the registered email address 
+4. User should be taken 'Reset your Password' page
+5. Success message with text - 'Success: Your password has been successfully updated.' should be displayed in green color and User should be navigated to 'Login' page
+6. User should be able to login with the new password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Application Email system is not working </t>
+  </si>
+  <si>
+    <t>Unable to test as the application email system in not working .</t>
+  </si>
+  <si>
+    <t>1. An email should be recevied by the registered email address with the details of resetting the password.
+2. Email should contain proper Subject, Body, from address and the link for resetting the password</t>
+  </si>
+  <si>
+    <t>Unable to test as the application email system in not working.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User should not be able to login with old password </t>
+  </si>
+  <si>
+    <t>1. User should be able to login</t>
+  </si>
+  <si>
+    <t>1. Success message with text - 'An email with a confirmation link has been sent your email address.' should be displayed in green color</t>
+  </si>
+  <si>
+    <t>1. Success message with text - 'An email with a confirmation link has been sent your email address.' is displayed in green color</t>
+  </si>
+  <si>
+    <t>1. User should be allowed to use the link sent in the email for resetting the password only once</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unable to test as the application email system in not working. </t>
+  </si>
+  <si>
+    <t>1. A field level warning message with text - 'Password and password confirmation do not match!' should be displayed under 'confirm' field</t>
+  </si>
+  <si>
+    <t>1. Proper placeholder texts are displayed inside the 'Password' and 'Confirm' fields of the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Field level warning message with text - 'Password must be between 4 and 20 characters!' should be displayed for 'Password' field</t>
+  </si>
+  <si>
+    <t>1. 'Right Columns' options should be displayed in the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. A proper working Breadcrumb should be displayed on the 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. A proper Page Heading, Page URL and Page Title should be displayed for 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for 'Reset your Password' page</t>
+  </si>
+  <si>
+    <t>1. Field level warning message with text - E-Mail must be between 4 and 20 characters!' should be displayed for 'E-Mail Address' field</t>
+  </si>
+  <si>
+    <t>1. Field level warning message with text - E-Mail must be between 4 and 20 characters!' is displayed for 'E-Mail Address' field</t>
+  </si>
+  <si>
+    <t>1. Proper Placeholder text is displayed inside the 'E-Mail Address' fields  of the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. 'E-Mail' Address field in the 'Forgotten Password' page should be marked as mandatory</t>
+  </si>
+  <si>
+    <t>1. 'E-Mail' Address field in the 'Forgotten Password' page is marked as mandatory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Try all below invalid email address formats:
+1) pavanol
+2) pavanol@
+3) pavanol@gmail
+4) pavanol@gmail.
+</t>
+  </si>
+  <si>
+    <t>1. Field level warning message informing the User to provide a valid formatted email address should be displayed</t>
+  </si>
+  <si>
+    <t>1. Field level warning message informing the User to provide a valid formatted email address is displayed</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Login' page</t>
+  </si>
+  <si>
+    <t>1. User is taken to 'Login' page</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to 'Forgotten Password page</t>
+  </si>
+  <si>
+    <t>1. User is navigated to 'Forgotten Password page</t>
+  </si>
+  <si>
+    <t>1. A proper working Breadcrumb should be displayed on the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. A proper working Breadcrumb is  displayed on the 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Forgotten Password' page and email address given in the Login page should be displayed in this page by default [Usability point of view]</t>
+  </si>
+  <si>
+    <t>1. User is taken to 'Forgotten Password' page and email address given in the Login page is not displayed in this page by default [Usability point of view]</t>
+  </si>
+  <si>
+    <t>OPENCART-BUG-12</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist is displayed for 'Forgotten Password' page</t>
+  </si>
+  <si>
+    <t>1. Text entered into the 'Password' and 'Confirmed' fields should be toggled to hide its visibility (i.e. * or . Symbols should be displayed)</t>
+  </si>
+  <si>
+    <t>1. Reset Password functionality should work correctly in all the supported environments</t>
   </si>
 </sst>
 </file>
@@ -1438,12 +1567,18 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1465,7 +1600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1483,11 +1618,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="4" tint="0.39997558519241921"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1538,7 +1697,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Login_Test_Cases" displayName="Login_Test_Cases" ref="A1:K25" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Login_Test_Cases" displayName="Login_Test_Cases" ref="A1:K25" totalsRowShown="0" headerRowDxfId="1">
   <autoFilter ref="A1:K25" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Test Case ID"/>
@@ -1558,7 +1717,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Registration_Process_Validation" displayName="Registration_Process_Validation" ref="A1:K29" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Registration_Process_Validation" displayName="Registration_Process_Validation" ref="A1:K29" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:K29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Test Case ID"/>
@@ -1951,7 +2110,7 @@
   </sheetPr>
   <dimension ref="E1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
@@ -2130,8 +2289,8 @@
   <dimension ref="A1:K25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2146,38 +2305,38 @@
     <col min="11" max="11" width="37.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2953,7 +3112,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2968,38 +3127,38 @@
     <col min="11" max="11" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -3905,43 +4064,43 @@
   <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>330</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -4306,6 +4465,514 @@
       </c>
       <c r="J13" t="s">
         <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364D5A06-8CA2-40F3-AD0B-30490194592F}">
+  <dimension ref="A1:F27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="C3" t="s">
+        <v>372</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>217</v>
+      </c>
+      <c r="F3" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C4" t="s">
+        <v>372</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>217</v>
+      </c>
+      <c r="F4" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>376</v>
+      </c>
+      <c r="C5" t="s">
+        <v>372</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>217</v>
+      </c>
+      <c r="F5" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>377</v>
+      </c>
+      <c r="C6" t="s">
+        <v>372</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" t="s">
+        <v>217</v>
+      </c>
+      <c r="F6" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>378</v>
+      </c>
+      <c r="C7" t="s">
+        <v>379</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>380</v>
+      </c>
+      <c r="C8" t="s">
+        <v>372</v>
+      </c>
+      <c r="D8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" t="s">
+        <v>217</v>
+      </c>
+      <c r="F8" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>382</v>
+      </c>
+      <c r="C9" t="s">
+        <v>372</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F9" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" t="s">
+        <v>383</v>
+      </c>
+      <c r="C10" t="s">
+        <v>372</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>384</v>
+      </c>
+      <c r="C11" t="s">
+        <v>372</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>217</v>
+      </c>
+      <c r="F11" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>264</v>
+      </c>
+      <c r="C12" t="s">
+        <v>372</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>217</v>
+      </c>
+      <c r="F12" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>385</v>
+      </c>
+      <c r="C13" t="s">
+        <v>372</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>217</v>
+      </c>
+      <c r="F13" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>386</v>
+      </c>
+      <c r="C14" t="s">
+        <v>372</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>217</v>
+      </c>
+      <c r="F14" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" t="s">
+        <v>387</v>
+      </c>
+      <c r="C15" t="s">
+        <v>372</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>217</v>
+      </c>
+      <c r="F15" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>388</v>
+      </c>
+      <c r="C16" t="s">
+        <v>372</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>217</v>
+      </c>
+      <c r="F16" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>389</v>
+      </c>
+      <c r="C17" t="s">
+        <v>390</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>391</v>
+      </c>
+      <c r="C18" t="s">
+        <v>391</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>392</v>
+      </c>
+      <c r="C19" t="s">
+        <v>393</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="B20" t="s">
+        <v>395</v>
+      </c>
+      <c r="C20" t="s">
+        <v>396</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>397</v>
+      </c>
+      <c r="C21" t="s">
+        <v>398</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>399</v>
+      </c>
+      <c r="C22" t="s">
+        <v>400</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>401</v>
+      </c>
+      <c r="C23" t="s">
+        <v>402</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>403</v>
+      </c>
+      <c r="C24" t="s">
+        <v>404</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B25" t="s">
+        <v>406</v>
+      </c>
+      <c r="C25" t="s">
+        <v>407</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>408</v>
+      </c>
+      <c r="C26" t="s">
+        <v>372</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" t="s">
+        <v>217</v>
+      </c>
+      <c r="F26" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>409</v>
+      </c>
+      <c r="C27" t="s">
+        <v>372</v>
+      </c>
+      <c r="D27" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" t="s">
+        <v>217</v>
+      </c>
+      <c r="F27" t="s">
+        <v>375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update E Commerce Project with Search funtion tcs
</commit_message>
<xml_diff>
--- a/01_BaseLine/BL01/E Commerce Project.xlsx
+++ b/01_BaseLine/BL01/E Commerce Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoang\E_Commerce_Test\01_BaseLine\BL01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E06ECE-660C-4D2A-B339-9D2D8FDCFFBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8FF673-59CD-4834-A991-526070FF2B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Register" sheetId="4" r:id="rId4"/>
     <sheet name="Logout" sheetId="5" r:id="rId5"/>
     <sheet name="Forgot Password" sheetId="6" r:id="rId6"/>
+    <sheet name="Search" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="410">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="455">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1546,6 +1547,162 @@
   </si>
   <si>
     <t>1. Reset Password functionality should work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>Product Name: iMac</t>
+  </si>
+  <si>
+    <t>1. Searched product should be displayed in the search results</t>
+  </si>
+  <si>
+    <t>1. Searched product is displayed in the search results</t>
+  </si>
+  <si>
+    <t>Product Name: Fitbit</t>
+  </si>
+  <si>
+    <t>1. 'There is no product that matches the search criteria' should be displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>1. 'There is no product that matches the search criteria' is displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>1.'There is no product that matches the search criteria' should be displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>Product Name: Mac</t>
+  </si>
+  <si>
+    <t>1. More than one products should be displayed in the search results page</t>
+  </si>
+  <si>
+    <t>1. More than one products are displayed in the search results page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Proper placeholder text is displayed in the below fields:
+- Search text box field
+- Search Criteria text box field
+</t>
+  </si>
+  <si>
+    <t>Text in Production description of iMac Product:  iLife</t>
+  </si>
+  <si>
+    <t>1. Product having the given text in its description should be displayed in the search results</t>
+  </si>
+  <si>
+    <t>1. Product having the given text in its description is displayed in the search results</t>
+  </si>
+  <si>
+    <t>Product Name: iMac
+Correct Category Name: Mac
+Wrong Category Name: PC</t>
+  </si>
+  <si>
+    <t>1. Product should be successfully displayed in the search results.
+2. 'There is no product that matches the search criteria' should be displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t>1. Product is successfully displayed in the search results.
+2. 'There is no product that matches the search criteria' is displayed in the Search Results page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Name: iMac
+Parent Category Name: Desktops
+</t>
+  </si>
+  <si>
+    <t>1. 'There is no product that matches the search criteria' should be displayed in the Search Results page
+2. Searched product should be displayed in the search results</t>
+  </si>
+  <si>
+    <t>1. 'There is no product that matches the search criteria' is displayed in the Search Results page
+2. Searched product is displayed in the search results</t>
+  </si>
+  <si>
+    <t>1. Single product should be dislayed in the List view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working 
+2. User should be navigated to the Product Display Page of the product
+3. Single product should be dislayed in the Grid view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working 
+4. User should be navigated to the Product Display Page of the product</t>
+  </si>
+  <si>
+    <t>Working as mentioned in the Actual results</t>
+  </si>
+  <si>
+    <t>Search Criteria: Mac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. More than one products should be displayed in the search results page
+2. Multiple product should be dislayed in the List view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working. Also User should be able to navigate to Product Displaye Page of products by clicking on Images and Product Name. 
+3. Multiple product should be dislayed in the Grid view without any problems and all the options (Add to Cart, Wish List and Compare Product) are working. Also User should be able to navigate to Product Displaye Page of products by clicking on Images and Product Name. 
+</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to the Product Compare Page</t>
+  </si>
+  <si>
+    <t>1. User is navigated to the Product Compare Page</t>
+  </si>
+  <si>
+    <t>1. More than one product should be displayed in the search results page
+2. Products are sorted according to the options selected in the 'Sort By' dropdown field</t>
+  </si>
+  <si>
+    <t>1. More than one product are  displayed in the search results page
+2. Products are sorted according to the options selected in the 'Sort By' dropdown field</t>
+  </si>
+  <si>
+    <t>1. More than one product should be displayed in the search results page
+2. The selected number of products should be displayed in the current search page</t>
+  </si>
+  <si>
+    <t>1. More than one product is displayed in the search results page
+2. The selected number of products are displayed in the current search page</t>
+  </si>
+  <si>
+    <t>1. Search box field and the button with 'Search' icon should be displayed on all the page of the Application</t>
+  </si>
+  <si>
+    <t>1. Search box field and the button with 'Search' icon are displayed on all the page of the Application</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to 'Search' page</t>
+  </si>
+  <si>
+    <t>1. User is navigated to 'Search' page</t>
+  </si>
+  <si>
+    <t>1. Breakcrumb option should be working correctly</t>
+  </si>
+  <si>
+    <t>1. Breakcrumb option is working correctly</t>
+  </si>
+  <si>
+    <t>1. User should be able to perform Search operation and select several options in the Search page using the Keyboard keys Tab and Enter</t>
+  </si>
+  <si>
+    <t>1.'Search in subcategories' option is not getting highlighted using the tab key</t>
+  </si>
+  <si>
+    <t>OPENCART-BUG-13</t>
+  </si>
+  <si>
+    <t>1. A proper Page Heading, Page URL and Page Title should be displayed for 'Search' page</t>
+  </si>
+  <si>
+    <t>1. A proper Page Heading, Page URL and Page Title are displayed for 'Search' page</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for the complete Search functionality</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist are displayed for the complete Search functionality</t>
+  </si>
+  <si>
+    <t>1. Search functionality should work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>1. Search functionality is working correctly in all the supported environments</t>
   </si>
 </sst>
 </file>
@@ -4476,7 +4633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{364D5A06-8CA2-40F3-AD0B-30490194592F}">
   <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -4978,4 +5135,416 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61EA799-E324-417F-BF2D-189B2797FFE5}">
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B3" t="s">
+        <v>411</v>
+      </c>
+      <c r="C3" t="s">
+        <v>412</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>413</v>
+      </c>
+      <c r="B4" t="s">
+        <v>414</v>
+      </c>
+      <c r="C4" t="s">
+        <v>415</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>416</v>
+      </c>
+      <c r="C5" t="s">
+        <v>415</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>410</v>
+      </c>
+      <c r="B6" t="s">
+        <v>411</v>
+      </c>
+      <c r="C6" t="s">
+        <v>412</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>417</v>
+      </c>
+      <c r="B7" t="s">
+        <v>418</v>
+      </c>
+      <c r="C7" t="s">
+        <v>419</v>
+      </c>
+      <c r="D7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C9" t="s">
+        <v>412</v>
+      </c>
+      <c r="D9" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>421</v>
+      </c>
+      <c r="B10" t="s">
+        <v>422</v>
+      </c>
+      <c r="C10" t="s">
+        <v>423</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
+        <v>424</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>425</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>426</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="5" t="s">
+        <v>427</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>429</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>410</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>430</v>
+      </c>
+      <c r="C13" t="s">
+        <v>431</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>432</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>433</v>
+      </c>
+      <c r="C14" t="s">
+        <v>431</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>410</v>
+      </c>
+      <c r="B15" t="s">
+        <v>434</v>
+      </c>
+      <c r="C15" t="s">
+        <v>435</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>417</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>436</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>437</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>417</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>439</v>
+      </c>
+      <c r="D17" t="s">
+        <v>39</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>440</v>
+      </c>
+      <c r="C18" t="s">
+        <v>441</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" t="s">
+        <v>442</v>
+      </c>
+      <c r="C19" t="s">
+        <v>443</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>410</v>
+      </c>
+      <c r="B20" t="s">
+        <v>444</v>
+      </c>
+      <c r="C20" t="s">
+        <v>445</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" t="s">
+        <v>446</v>
+      </c>
+      <c r="C21" t="s">
+        <v>447</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" t="s">
+        <v>449</v>
+      </c>
+      <c r="C22" t="s">
+        <v>450</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" t="s">
+        <v>451</v>
+      </c>
+      <c r="C23" t="s">
+        <v>452</v>
+      </c>
+      <c r="D23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" t="s">
+        <v>453</v>
+      </c>
+      <c r="C24" t="s">
+        <v>454</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Product Compare Testcases
</commit_message>
<xml_diff>
--- a/01_BaseLine/BL01/E Commerce Project.xlsx
+++ b/01_BaseLine/BL01/E Commerce Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoang\E_Commerce_Test\01_BaseLine\BL01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D8FF673-59CD-4834-A991-526070FF2B53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF50A9BE-A6B0-4E03-AE0D-5CA17A2F7E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3195" yWindow="3195" windowWidth="21600" windowHeight="11505" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Logout" sheetId="5" r:id="rId5"/>
     <sheet name="Forgot Password" sheetId="6" r:id="rId6"/>
     <sheet name="Search" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="964" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="493">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1703,6 +1704,137 @@
   </si>
   <si>
     <t>1. Search functionality is working correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Tool tip with the text - 'Compare this Product' should be displayed
+2. Success message with text - ' Success: You have added Product Name to your product comparison!' should be displayed
+3. User should be taken to the 'Product Comparison' page with the details of the Product that we have added for comparision. </t>
+  </si>
+  <si>
+    <t>Working exactly as per mentioned in the Expected Result setion</t>
+  </si>
+  <si>
+    <t>1. User should be taken to 'Product Compare' page</t>
+  </si>
+  <si>
+    <t>1. User is taken to 'Product Compare' page</t>
+  </si>
+  <si>
+    <t>1. 'You have not chosen any products to compare.' should be displayed on the page</t>
+  </si>
+  <si>
+    <t>1. 'You have not chosen any products to compare.' is displayed on the page</t>
+  </si>
+  <si>
+    <t>1. User should be navigated to 'Home' page</t>
+  </si>
+  <si>
+    <t>1. User is navigated to 'Home' page</t>
+  </si>
+  <si>
+    <t>1. Breadcrumb should work without any problems</t>
+  </si>
+  <si>
+    <t>1. Breadcrumb is working without any problems</t>
+  </si>
+  <si>
+    <t>1. Success message with text - ' Success: You have added Product Name to your product comparison!' should be displayed
+2. User should be navigated to the respective Product Display Page
+3. User shluld be taken to the 'Prdocut Comparison' page</t>
+  </si>
+  <si>
+    <t>1. Success message with text - ' Success: You have added Product Name to your product comparison!' is displayed
+2. User is navigated to the respective Product Display Page
+3. User should be taken to the 'Product Comparison' page</t>
+  </si>
+  <si>
+    <t>1. Validate that a single product is displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t>1. A single product is displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t>Product Name: iMac
+Any other Product Name: iPhone</t>
+  </si>
+  <si>
+    <t>1. Validate that two products are displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t>1. Two products are displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Name: iMac
+</t>
+  </si>
+  <si>
+    <t>1. Validate that the product shoud be displayed in the 'Product Comparison' page only one with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t>1. Single product shoud be displayed in the 'Product Comparison' page only one with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t>First Product Name: iMac
+Second Product Name: iPhone
+Third Product Name: MacBook Air</t>
+  </si>
+  <si>
+    <t>1. Validate that three products are displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t>Three products are displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t>First Product Name: iMac
+Second Product Name: iPhone
+Third Product Name: MacBook Air
+Fourth Product Name: MacBook</t>
+  </si>
+  <si>
+    <t>1. Validate that four products are displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t>1. Four products are displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons)</t>
+  </si>
+  <si>
+    <t>First Product Name: iMac
+Second Product Name: iPhone
+Third Product Name: MacBook Air
+Fourth Product Name: MacBook
+Fifth Product Name: MacBook Pro</t>
+  </si>
+  <si>
+    <t>1. Validate that lastest four products (Second Product Name to Fifth Product Name) are displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons) and the First added Product is automatically removed from the 'Product Comparison' page as it allows only four products for comparision.</t>
+  </si>
+  <si>
+    <t>1. Lastest four products (Second Product Name to Fifth Product Name) are displayed in the 'Product Comparison' page with all the proper product details and the buttons (Add to Cart and Remove buttons) and the First added Product is automatically removed from the 'Product Comparison' page as it allows only four products for comparision.</t>
+  </si>
+  <si>
+    <t>1. Validate that the products are successfully added to the 'Shopping Cart' page from the 'Product Compare' page. Check this by also adding mulitple products to the 'Product Comparison' page.</t>
+  </si>
+  <si>
+    <t>1. Products are successfully added to the 'Shopping Cart' page from the 'Product Compare' page.</t>
+  </si>
+  <si>
+    <t>1. Validate that the products are successfully removed from the 'Product Compare' page. Check this by adding and removing mulitple products to the 'Product Comparison' page.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Products are successfully removed from the 'Product Compare' page. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Proper Page Title, Page Heading and Page URL of the 'Product Comparison' page are displayed. </t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for the complete 'Product Comparison' functionality</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist is  displayed for the complete 'Product Comparison' functionality</t>
+  </si>
+  <si>
+    <t>1. 'Product  Comparison' functionality should work correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>1. 'Product  Comparison' functionality is working correctly in all the supported environments</t>
   </si>
 </sst>
 </file>
@@ -4987,7 +5119,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="242.25" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>394</v>
       </c>
@@ -5141,7 +5273,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C61EA799-E324-417F-BF2D-189B2797FFE5}">
   <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F24"/>
     </sheetView>
   </sheetViews>
@@ -5547,4 +5679,447 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4874D30F-1607-4E22-BBFB-C5733DC32EDB}">
+  <dimension ref="A1:F26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C3" t="s">
+        <v>456</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>410</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C4" t="s">
+        <v>456</v>
+      </c>
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>410</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C5" t="s">
+        <v>456</v>
+      </c>
+      <c r="D5" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C6" t="s">
+        <v>456</v>
+      </c>
+      <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C7" t="s">
+        <v>456</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>410</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C8" t="s">
+        <v>456</v>
+      </c>
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C9" t="s">
+        <v>456</v>
+      </c>
+      <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>410</v>
+      </c>
+      <c r="B10" t="s">
+        <v>457</v>
+      </c>
+      <c r="C10" t="s">
+        <v>458</v>
+      </c>
+      <c r="D10" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" t="s">
+        <v>457</v>
+      </c>
+      <c r="C11" t="s">
+        <v>458</v>
+      </c>
+      <c r="D11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" t="s">
+        <v>459</v>
+      </c>
+      <c r="C12" t="s">
+        <v>460</v>
+      </c>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>461</v>
+      </c>
+      <c r="C13" t="s">
+        <v>462</v>
+      </c>
+      <c r="D13" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>463</v>
+      </c>
+      <c r="C14" t="s">
+        <v>464</v>
+      </c>
+      <c r="D14" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>410</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>465</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>466</v>
+      </c>
+      <c r="D15" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>410</v>
+      </c>
+      <c r="B16" t="s">
+        <v>467</v>
+      </c>
+      <c r="C16" t="s">
+        <v>468</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="5" t="s">
+        <v>469</v>
+      </c>
+      <c r="B17" t="s">
+        <v>470</v>
+      </c>
+      <c r="C17" t="s">
+        <v>471</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B18" t="s">
+        <v>473</v>
+      </c>
+      <c r="C18" t="s">
+        <v>474</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="5" t="s">
+        <v>475</v>
+      </c>
+      <c r="B19" t="s">
+        <v>476</v>
+      </c>
+      <c r="C19" t="s">
+        <v>477</v>
+      </c>
+      <c r="D19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="242.25" x14ac:dyDescent="0.2">
+      <c r="A20" s="5" t="s">
+        <v>478</v>
+      </c>
+      <c r="B20" t="s">
+        <v>479</v>
+      </c>
+      <c r="C20" t="s">
+        <v>480</v>
+      </c>
+      <c r="D20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="313.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="B21" t="s">
+        <v>482</v>
+      </c>
+      <c r="C21" t="s">
+        <v>483</v>
+      </c>
+      <c r="D21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A22" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B22" t="s">
+        <v>484</v>
+      </c>
+      <c r="C22" t="s">
+        <v>485</v>
+      </c>
+      <c r="D22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A23" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B23" t="s">
+        <v>486</v>
+      </c>
+      <c r="C23" t="s">
+        <v>487</v>
+      </c>
+      <c r="D23" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A24" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B24" t="s">
+        <v>488</v>
+      </c>
+      <c r="C24" t="s">
+        <v>488</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A25" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B25" t="s">
+        <v>489</v>
+      </c>
+      <c r="C25" t="s">
+        <v>490</v>
+      </c>
+      <c r="D25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="57" x14ac:dyDescent="0.2">
+      <c r="A26" s="5" t="s">
+        <v>472</v>
+      </c>
+      <c r="B26" t="s">
+        <v>491</v>
+      </c>
+      <c r="C26" t="s">
+        <v>492</v>
+      </c>
+      <c r="D26" t="s">
+        <v>27</v>
+      </c>
+      <c r="E26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update E Commerce Project spreadsheet with Product Display Test cases
</commit_message>
<xml_diff>
--- a/01_BaseLine/BL01/E Commerce Project.xlsx
+++ b/01_BaseLine/BL01/E Commerce Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoang\E_Commerce_Test\01_BaseLine\BL01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF50A9BE-A6B0-4E03-AE0D-5CA17A2F7E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F160962A-EBB7-4FAC-BB16-3E2DC527B673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3195" yWindow="3195" windowWidth="21600" windowHeight="11505" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="3540" windowWidth="21600" windowHeight="11505" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version History" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,8 @@
     <sheet name="Logout" sheetId="5" r:id="rId5"/>
     <sheet name="Forgot Password" sheetId="6" r:id="rId6"/>
     <sheet name="Search" sheetId="7" r:id="rId7"/>
-    <sheet name="Sheet1" sheetId="8" r:id="rId8"/>
+    <sheet name="Product Compare" sheetId="8" r:id="rId8"/>
+    <sheet name="Product Display Page" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1090" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="648">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -1835,6 +1836,613 @@
   </si>
   <si>
     <t>1. 'Product  Comparison' functionality is working correctly in all the supported environments</t>
+  </si>
+  <si>
+    <t>TC_PDP_001</t>
+  </si>
+  <si>
+    <t>(TS_007)
+Product Display Page</t>
+  </si>
+  <si>
+    <t>Validate the Thumbnails of the Product displayed in the Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on the main bigger sized Thumbnail image displayed on the 'Product Display Page' (Validate ER-1)
+5. Click on '&lt;' and '&gt;' options (Validate ER-2)
+6. Click on 'x' option or press 'ESC' keyboard key when the thumbnails are displayed in Light box view (Validate ER-3)
+7. Click on the normal sized Thumbnail images and repeat the steps 5 to 6 (Validate ER-4)</t>
+  </si>
+  <si>
+    <t>1. Light box view of the main Thumnail image should be displayed with options to view the previous and next Thumnail images in Light box view.
+2. User should be able to navigate to other thumbnail images in the Light box view 
+3. Light box view should close and the focus should go to the Product Display Page.
+4 Light box view of the selected Thumnail image should be displayed with options to view the previous and next Thumnail images in Light box view.  User should be able to navigate to other thumbnail images in the Light box view. Light box view should close and the focus should go to the Product Display Page.</t>
+  </si>
+  <si>
+    <t>Working as mentioned in the Expected Result section</t>
+  </si>
+  <si>
+    <t>TC_PDP_002</t>
+  </si>
+  <si>
+    <t>Validate that Product Name, Brand and Product Code are displayed in the Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the Product Name, Brand and Product Code in the displayed Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Proper Product Name, Brand and Product Code should be displayed for the different types of Products in the Product Display Page.</t>
+  </si>
+  <si>
+    <t>Proper Product Name, Brand and Product Code are displayed for the different types of Products in the Product Display Page.</t>
+  </si>
+  <si>
+    <t>TC_PDP_003</t>
+  </si>
+  <si>
+    <t>Validate the availabilty status of the Product in the Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the different availability status of the Products in the displayed Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Proper avaialabilty statuses like In Stock, Out of Stock and Limited Stock should be displayed in the Availabilty section of the Product Display Page for the different types of Products.</t>
+  </si>
+  <si>
+    <t>Proper avaialabilty statuses like In Stock, Out of Stock and Limited Stock are displayed in the Availabilty section of the Product Display Page for the different types of Products.</t>
+  </si>
+  <si>
+    <t>TC_PDP_004</t>
+  </si>
+  <si>
+    <t>Validate the Price of the Product with and without tax is displayed in the Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the Price with tax and Price Ex Tax in the displayed Product Display Page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper price with and without tax should be displayed for the different types of Products in the Product Display Page.</t>
+  </si>
+  <si>
+    <t>Proper price with and without tax is displayed for the different types of Products in the Product Display Page.</t>
+  </si>
+  <si>
+    <t>TC_PDP_005</t>
+  </si>
+  <si>
+    <t>Validate the default quanity for the Product is displayed as 1 in the Product Display Page, when there is no minimum quantity set for the Product</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field, which has no minimum quanitity set - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the Qty text field in the Product Display Page (Validate ER-1)
+5. Update the quantity by increasing it to more than one and click on 'Add to Cart' button (Validate ER-2)</t>
+  </si>
+  <si>
+    <t>1. Default quantity should be displayed 1 for this product which has not minimum quantity set
+2. Quantity should get updated accordingly and the User should be able to add the Product to cart without any issues.</t>
+  </si>
+  <si>
+    <t>TC_PDP_006</t>
+  </si>
+  <si>
+    <t>Validate the negative quantity or zero quantity or null quantity should not be allowed in the Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field, which has no minimum quanitity set - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the Qty text field in the Product Display Page
+5. Update the quantity in the Qty text feild by providing a negative number or zero number or null quanitity and click on 'Add to Cart' button  (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. A field level message - 'Quantity should be a positive number' or 'Quantity cannot be zero, null or negative' should be displayed under the Qty text field</t>
+  </si>
+  <si>
+    <t>Warning messsage is not getting displayed</t>
+  </si>
+  <si>
+    <t>OPENCART-BUG-14</t>
+  </si>
+  <si>
+    <t>TC_PDP_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the Product having the minimum quanitity set </t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field, which has no minimum quanitity set - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the Qty text field in the Product Display Page (Validate ER-1)
+5. Fill all the mandatory fields in the Product Display Page of this product and reduce below the minimum quantity in the Qty text feild and click on 'Add to Cart' button and navigate to shopping cart page (Validate ER-2)
+6. Increase the Quantity in the Qty field to more than the minimum quantity and click on 'Add to Cart' button (Validate ER-3)</t>
+  </si>
+  <si>
+    <t>Product Name: Apple Cinema 30"</t>
+  </si>
+  <si>
+    <t>1. Default quantity in Qty field should be displayed as minimum quanity set for this product (This product has minimum quanity set as 2). Also, the information text - ' This product has a minimum quantity of 2' should be displayed under the 'Add to Cart' button 
+2. Warning message stating - 'Minimum order amount for Apple Cinema 30" is 2!'
+3. Product should be added to the cart with the given quantity without any problems.</t>
+  </si>
+  <si>
+    <t>TC_PDP_008</t>
+  </si>
+  <si>
+    <t>Validate the description of the Product in the Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on the Description tab of the Product in the displayed 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Correct Description of the product without any spelling or grammatical mistakes should be displayed for different types of Products.</t>
+  </si>
+  <si>
+    <t>TC_PDP_009</t>
+  </si>
+  <si>
+    <t>Validate the specifications of the Product in the Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on the Specification tab of the Product in the displayed 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Correct Specifications of the product without any spelling or grammatrical mistakes should be displayed for different types of Products.</t>
+  </si>
+  <si>
+    <t>TC_PDP_010</t>
+  </si>
+  <si>
+    <t>Validate the User is able to write a review for the Product from the 'Reviews' tab of Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on the Reviews tab of the Product in the displayed 'Product Display' page
+5. Enter your name into the 'Your Name' text field
+6. Enter review text into the 'Your Review' text are field
+7. Select any radio button to give the rating
+8. Click on 'Continue' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Success message with text - 'Thank you for your review. It has been submitted to the webmaster for approval.' should be displayed. This review should be displayed under this 'Reviews' tab once the webmaster approves it.</t>
+  </si>
+  <si>
+    <t>TC_PDP_011</t>
+  </si>
+  <si>
+    <t>Validate the 'Reviews' tab when there are no reviews or zero reviews added</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field for which there are no existing reviews - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on the Reviews(0) tab of the Product in the displayed 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. 'There are no reviews for this product.' text should be displayed under the 'Reviews' tab</t>
+  </si>
+  <si>
+    <t>TC_PDP_012</t>
+  </si>
+  <si>
+    <t>Validate all the fields in the 'Review' tab are mandatory fields</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on the Reviews tab of the Product in the displayed 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. All the fields in the Reviews tab should be mandatory fields.</t>
+  </si>
+  <si>
+    <t>TC_PDP_013</t>
+  </si>
+  <si>
+    <t>Validate 'Write a review' link under 'Add to Cart' button on the 'Product Display' page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on 'Write a review' link under 'Add to Cart' button of the 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. 'Reviews' tab in the Product Display page should come to the focus.</t>
+  </si>
+  <si>
+    <t>TC_PDP_014</t>
+  </si>
+  <si>
+    <t>Validate average of the user reviews should be dispalyed under the 'Add to Cart' button of the Product Display page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the average and number of reviews under the 'Add to Cart' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Correct average review and the number of reviews count should be displayed under the 'Add to Cart' button</t>
+  </si>
+  <si>
+    <t>TC_PDP_015</t>
+  </si>
+  <si>
+    <t>Validate the count of reviews should be displayed in the 'Reviews' tab label of the Product Display page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the count of reviews in the 'Reviews' tab lable in the Product Display page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Correct count of reviews should be displayed in the 'Reviews' tab label of the Product Display Page</t>
+  </si>
+  <si>
+    <t>TC_PDP_016</t>
+  </si>
+  <si>
+    <t>Validate 'reviews' link under the 'Add to Cart' button of Product Display Page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on the 'x reviews' link in the Product Display page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Reviews given the User so far should be displayed under the 'Reviews' tab of the Product Display Page.</t>
+  </si>
+  <si>
+    <t>TC_PDP_017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate submitting a review without filling the mandatory fields </t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Select the Reviews tab of the Product in the displayed 'Product Display' page 
+5. Don't provide Name, Your Review and Ratings and click on 'Continue' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper warning messages informing the User to fill the mandatory fields to submit the review should be displayed.</t>
+  </si>
+  <si>
+    <t>TC_PDP_018</t>
+  </si>
+  <si>
+    <t>Validate the review text given while writing is accepted according to the specified number of characters</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Select the Reviews tab of the Product in the displayed 'Product Display' page 
+5. Provide Name and Ratings
+6. Check whether a proper warning message is displayed on providing the review text which is not according to the specified range of characters (i.e. 25 to 100 charactres) and click on 'Continue' button (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper warning message with the text - 'Warning: Review Text must be between 25 and 1000 characters!' should be displayed</t>
+  </si>
+  <si>
+    <t>TC_PDP_019</t>
+  </si>
+  <si>
+    <t>Validate adding the product to 'Wish List' from the Product Display page</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL and Login</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on 'Add to Wish List' option in the displayed 'Product Display' page (Validate ER-1)
+5. Click on 'wish list' link in the success message (Validate ER-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Success message with text - 'Success: You have added Product Name to your wish list!' is displayed
+2. User should be taken to 'Wish List page and the product added is displayed in the 'Wish List' page
+</t>
+  </si>
+  <si>
+    <t>TC_PDP_020</t>
+  </si>
+  <si>
+    <t>Validate adding the product for comparision from the Product Display page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL </t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on 'Compare this Product' option in the displayed 'Product Display' page (Validate ER-1)
+5. Click on 'product comparisoin' link in the success message (Validate ER-2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Success message with text - ' Success: You have added Product Name to your product comparison!' is displayed
+2. User should be taken to 'Product Comparison' page and the product details are displayed in the page
+</t>
+  </si>
+  <si>
+    <t>TC_PDP_021</t>
+  </si>
+  <si>
+    <t>Validate proper options for liking, tweeting, sharing the Product Display page on social platforms</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the options for liking, tweeting, sharing the Product Display page on social platforms (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be able to like, tweet, share the Product Display page on social platforms</t>
+  </si>
+  <si>
+    <t>TC_PDP_022</t>
+  </si>
+  <si>
+    <t>Validate 'Related Products' section in Product Display page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on the 'Related Products' section in the displayed Product Display Page</t>
+  </si>
+  <si>
+    <t>1. User should see the Product displayed in the 'Related Products' section and is able ot click it and navigate to the Product Display Page of it.</t>
+  </si>
+  <si>
+    <t>TC_PDP_023</t>
+  </si>
+  <si>
+    <t>Validate navigating to the Product Display page by using the Product image in the 'Wish List' page</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL and Login
+2.A product is added to the Wish List page</t>
+  </si>
+  <si>
+    <t>1. Click on the 'Wish List' header option
+2. Click on the Image icon displayed under the 'Image' section of the displayed 'Wish List' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be taken the Product Display page of the Product that is displayed in the 'Wish List' page</t>
+  </si>
+  <si>
+    <t>TC_PDP_024</t>
+  </si>
+  <si>
+    <t>Validate navigating to the Product Display page by using the Product Name link in the 'Wish List' page</t>
+  </si>
+  <si>
+    <t>1. Click on the 'Wish List' header option
+2. Click on the Product Name link displayed under the 'Product Name' section of the displayed 'Wish List' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. User should be taken to the Product Display page of the Product that is displayed in the 'Wish List' page</t>
+  </si>
+  <si>
+    <t>TC_PDP_025</t>
+  </si>
+  <si>
+    <t>Validate navigating to the Product Display page by using the Product Name link in Success message on adding the Product to Cart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL and Login
+</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on 'Add to Cart' button
+5. Click on 'Product Name' link from the displayed success page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User should be taken to the Product Display page of the Product </t>
+  </si>
+  <si>
+    <t>TC_PDP_026</t>
+  </si>
+  <si>
+    <t>Validate navigating to the Product Display page by using the Product Image in the 'Shopping Cart' page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on 'Add to Cart' button
+5. Click on 'shopping cart!' link from the displayed success page
+6. Click on the Product image from the displayed Shopping Cart page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>TC_PDP_027</t>
+  </si>
+  <si>
+    <t>Validate navigating to the Product Display page by using the Product Name link in the 'Shopping Cart' page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on 'Add to Cart' button
+5. Click on 'shopping cart!' link from the displayed success page
+6. Click on the Product Name link from the displayed Shopping Cart page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>TC_PDP_028</t>
+  </si>
+  <si>
+    <t>Validate navigating to the Product Display page by using the Product Name link in the 'Confirm Order' sectioon of the 'Checkout' page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Click on 'Add to Cart' button
+5. Click on 'Checkout' button in the displayed 'Shopping Cart' page
+6. Click on 'Continue' buttons and select any mandatory checkboxes until you reach the 'Confirm Order' section 
+7. Click on 'Product Name' link in the 'Confirm Order' section (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>TC_PDP_029</t>
+  </si>
+  <si>
+    <t>Validate navigating to the Product Display page by using the Product Image in the 'Cart' button toggle box</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on 'Add to Cart' option on the product that is displayed in the Search Results 
+4. Click on 'Cart' button which is in black color beside the search icon button on the top of the page
+5. Click on the Product Image in the displayed toggle box (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>TC_PDP_030</t>
+  </si>
+  <si>
+    <t>Validate navigating to the Product Display page by using the Product Name link in the 'Cart' button toggle box</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on 'Add to Cart' option on the product that is displayed in the Search Results 
+4. Click on 'Cart' button which is in black color beside the search icon button on the top of the page
+5. Click on the Product Name link in the displayed toggle box (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>TC_PDP_031</t>
+  </si>
+  <si>
+    <t>Validate the Reward Points displayed in the Product Display page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the 'Reward Points' in the displayed 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Correct rewards points should be displayed</t>
+  </si>
+  <si>
+    <t>TC_PDP_032</t>
+  </si>
+  <si>
+    <t>Validate the original price of the Product without offer in the Product Display page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the original price of the Product without offer in the displayed 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Orignal price should be displayed as striked off</t>
+  </si>
+  <si>
+    <t>TC_PDP_033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate the prices of the Product when purchased in bulk </t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the prices of the Product when purchased in bluk in the displayed 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Prices when purchased in bluk should be displayed correctly for 10 products, 20 products and 30 products </t>
+  </si>
+  <si>
+    <t>TC_PDP_034</t>
+  </si>
+  <si>
+    <t>Validate all the extra available options in the Product Display page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check all the 'Available Options'  in the displayed 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. User should be able to select all the available options </t>
+  </si>
+  <si>
+    <t>TC_PDP_035</t>
+  </si>
+  <si>
+    <t>Validate Page Title, Page Heading and Page URL of the 'Product Display' page</t>
+  </si>
+  <si>
+    <t>1. Open the Application URL in any supported browser</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field  - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results
+4. Check the Page Title, Page Heading and Page URL of hte displayed 'Product Display' page (Validate ER-1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Proper Page Title, Page Heading and Page URL of the 'Product Display' page are displayed. </t>
+  </si>
+  <si>
+    <t>TC_PDP_036</t>
+  </si>
+  <si>
+    <t>Validate the UI of 'Product Display' page</t>
+  </si>
+  <si>
+    <t>1. Enter any existing Product name into the Search text box field - &lt;Refer Test Data&gt;
+2. Click on the button having search icon
+3. Click on the Product displayed in the Search results (Validate ER-1)</t>
+  </si>
+  <si>
+    <t>1. Proper UI adhering to the UI checklist should be displayed for the complete 'Product Display' page functionality</t>
+  </si>
+  <si>
+    <t>TC_PDP_037</t>
+  </si>
+  <si>
+    <t>Validate the 'Product Display' page functionality in all the supported environments</t>
+  </si>
+  <si>
+    <t>1. 'Product  Display' page functionality should work correctly in all the supported environments</t>
   </si>
 </sst>
 </file>
@@ -1918,7 +2526,35 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1986,7 +2622,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Login_Test_Cases" displayName="Login_Test_Cases" ref="A1:K25" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Login_Test_Cases" displayName="Login_Test_Cases" ref="A1:K25" totalsRowShown="0" headerRowDxfId="5">
   <autoFilter ref="A1:K25" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Test Case ID"/>
@@ -2006,7 +2642,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Registration_Process_Validation" displayName="Registration_Process_Validation" ref="A1:K29" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Registration_Process_Validation" displayName="Registration_Process_Validation" ref="A1:K29" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="A1:K29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="Test Case ID"/>
@@ -5685,8 +6321,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4874D30F-1607-4E22-BBFB-C5733DC32EDB}">
   <dimension ref="A1:F26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -6122,4 +6758,1246 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB4AD56-6110-49EF-84B3-346738C4C6E9}">
+  <dimension ref="A1:K39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B3" t="s">
+        <v>494</v>
+      </c>
+      <c r="C3" t="s">
+        <v>495</v>
+      </c>
+      <c r="D3" t="s">
+        <v>348</v>
+      </c>
+      <c r="E3" t="s">
+        <v>496</v>
+      </c>
+      <c r="F3" t="s">
+        <v>410</v>
+      </c>
+      <c r="G3" t="s">
+        <v>497</v>
+      </c>
+      <c r="H3" t="s">
+        <v>498</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>499</v>
+      </c>
+      <c r="B4" t="s">
+        <v>494</v>
+      </c>
+      <c r="C4" t="s">
+        <v>500</v>
+      </c>
+      <c r="D4" t="s">
+        <v>348</v>
+      </c>
+      <c r="E4" t="s">
+        <v>501</v>
+      </c>
+      <c r="F4" t="s">
+        <v>410</v>
+      </c>
+      <c r="G4" t="s">
+        <v>502</v>
+      </c>
+      <c r="H4" t="s">
+        <v>503</v>
+      </c>
+      <c r="I4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>504</v>
+      </c>
+      <c r="B5" t="s">
+        <v>494</v>
+      </c>
+      <c r="C5" t="s">
+        <v>505</v>
+      </c>
+      <c r="D5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E5" t="s">
+        <v>506</v>
+      </c>
+      <c r="F5" t="s">
+        <v>410</v>
+      </c>
+      <c r="G5" t="s">
+        <v>507</v>
+      </c>
+      <c r="H5" t="s">
+        <v>508</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>509</v>
+      </c>
+      <c r="B6" t="s">
+        <v>494</v>
+      </c>
+      <c r="C6" t="s">
+        <v>510</v>
+      </c>
+      <c r="D6" t="s">
+        <v>348</v>
+      </c>
+      <c r="E6" t="s">
+        <v>511</v>
+      </c>
+      <c r="F6" t="s">
+        <v>410</v>
+      </c>
+      <c r="G6" t="s">
+        <v>512</v>
+      </c>
+      <c r="H6" t="s">
+        <v>513</v>
+      </c>
+      <c r="I6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>514</v>
+      </c>
+      <c r="B7" t="s">
+        <v>494</v>
+      </c>
+      <c r="C7" t="s">
+        <v>515</v>
+      </c>
+      <c r="D7" t="s">
+        <v>348</v>
+      </c>
+      <c r="E7" t="s">
+        <v>516</v>
+      </c>
+      <c r="F7" t="s">
+        <v>410</v>
+      </c>
+      <c r="G7" t="s">
+        <v>517</v>
+      </c>
+      <c r="H7" t="s">
+        <v>498</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
+      </c>
+      <c r="J7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>518</v>
+      </c>
+      <c r="B8" t="s">
+        <v>494</v>
+      </c>
+      <c r="C8" t="s">
+        <v>519</v>
+      </c>
+      <c r="D8" t="s">
+        <v>348</v>
+      </c>
+      <c r="E8" t="s">
+        <v>520</v>
+      </c>
+      <c r="F8" t="s">
+        <v>410</v>
+      </c>
+      <c r="G8" t="s">
+        <v>521</v>
+      </c>
+      <c r="H8" t="s">
+        <v>522</v>
+      </c>
+      <c r="I8" t="s">
+        <v>39</v>
+      </c>
+      <c r="J8" t="s">
+        <v>28</v>
+      </c>
+      <c r="K8" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>524</v>
+      </c>
+      <c r="B9" t="s">
+        <v>494</v>
+      </c>
+      <c r="C9" t="s">
+        <v>525</v>
+      </c>
+      <c r="D9" t="s">
+        <v>348</v>
+      </c>
+      <c r="E9" t="s">
+        <v>526</v>
+      </c>
+      <c r="F9" t="s">
+        <v>527</v>
+      </c>
+      <c r="G9" t="s">
+        <v>528</v>
+      </c>
+      <c r="H9" t="s">
+        <v>498</v>
+      </c>
+      <c r="I9" t="s">
+        <v>39</v>
+      </c>
+      <c r="J9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>529</v>
+      </c>
+      <c r="B10" t="s">
+        <v>494</v>
+      </c>
+      <c r="C10" t="s">
+        <v>530</v>
+      </c>
+      <c r="D10" t="s">
+        <v>348</v>
+      </c>
+      <c r="E10" t="s">
+        <v>531</v>
+      </c>
+      <c r="F10" t="s">
+        <v>410</v>
+      </c>
+      <c r="G10" t="s">
+        <v>532</v>
+      </c>
+      <c r="H10" t="s">
+        <v>498</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+      <c r="J10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>533</v>
+      </c>
+      <c r="B11" t="s">
+        <v>494</v>
+      </c>
+      <c r="C11" t="s">
+        <v>534</v>
+      </c>
+      <c r="D11" t="s">
+        <v>348</v>
+      </c>
+      <c r="E11" t="s">
+        <v>535</v>
+      </c>
+      <c r="F11" t="s">
+        <v>527</v>
+      </c>
+      <c r="G11" t="s">
+        <v>536</v>
+      </c>
+      <c r="H11" t="s">
+        <v>498</v>
+      </c>
+      <c r="I11" t="s">
+        <v>39</v>
+      </c>
+      <c r="J11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>537</v>
+      </c>
+      <c r="B12" t="s">
+        <v>494</v>
+      </c>
+      <c r="C12" t="s">
+        <v>538</v>
+      </c>
+      <c r="D12" t="s">
+        <v>348</v>
+      </c>
+      <c r="E12" t="s">
+        <v>539</v>
+      </c>
+      <c r="F12" t="s">
+        <v>527</v>
+      </c>
+      <c r="G12" t="s">
+        <v>540</v>
+      </c>
+      <c r="H12" t="s">
+        <v>498</v>
+      </c>
+      <c r="I12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>541</v>
+      </c>
+      <c r="B13" t="s">
+        <v>494</v>
+      </c>
+      <c r="C13" t="s">
+        <v>542</v>
+      </c>
+      <c r="D13" t="s">
+        <v>348</v>
+      </c>
+      <c r="E13" t="s">
+        <v>543</v>
+      </c>
+      <c r="F13" t="s">
+        <v>410</v>
+      </c>
+      <c r="G13" t="s">
+        <v>544</v>
+      </c>
+      <c r="H13" t="s">
+        <v>498</v>
+      </c>
+      <c r="I13" t="s">
+        <v>39</v>
+      </c>
+      <c r="J13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>545</v>
+      </c>
+      <c r="B14" t="s">
+        <v>494</v>
+      </c>
+      <c r="C14" t="s">
+        <v>546</v>
+      </c>
+      <c r="D14" t="s">
+        <v>348</v>
+      </c>
+      <c r="E14" t="s">
+        <v>547</v>
+      </c>
+      <c r="F14" t="s">
+        <v>410</v>
+      </c>
+      <c r="G14" t="s">
+        <v>548</v>
+      </c>
+      <c r="H14" t="s">
+        <v>498</v>
+      </c>
+      <c r="I14" t="s">
+        <v>39</v>
+      </c>
+      <c r="J14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>549</v>
+      </c>
+      <c r="B15" t="s">
+        <v>494</v>
+      </c>
+      <c r="C15" t="s">
+        <v>550</v>
+      </c>
+      <c r="D15" t="s">
+        <v>348</v>
+      </c>
+      <c r="E15" t="s">
+        <v>551</v>
+      </c>
+      <c r="F15" t="s">
+        <v>410</v>
+      </c>
+      <c r="G15" t="s">
+        <v>552</v>
+      </c>
+      <c r="H15" t="s">
+        <v>498</v>
+      </c>
+      <c r="I15" t="s">
+        <v>39</v>
+      </c>
+      <c r="J15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>553</v>
+      </c>
+      <c r="B16" t="s">
+        <v>494</v>
+      </c>
+      <c r="C16" t="s">
+        <v>554</v>
+      </c>
+      <c r="D16" t="s">
+        <v>348</v>
+      </c>
+      <c r="E16" t="s">
+        <v>555</v>
+      </c>
+      <c r="F16" t="s">
+        <v>410</v>
+      </c>
+      <c r="G16" t="s">
+        <v>556</v>
+      </c>
+      <c r="H16" t="s">
+        <v>498</v>
+      </c>
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>557</v>
+      </c>
+      <c r="B17" t="s">
+        <v>494</v>
+      </c>
+      <c r="C17" t="s">
+        <v>558</v>
+      </c>
+      <c r="D17" t="s">
+        <v>348</v>
+      </c>
+      <c r="E17" t="s">
+        <v>559</v>
+      </c>
+      <c r="F17" t="s">
+        <v>410</v>
+      </c>
+      <c r="G17" t="s">
+        <v>560</v>
+      </c>
+      <c r="H17" t="s">
+        <v>498</v>
+      </c>
+      <c r="I17" t="s">
+        <v>39</v>
+      </c>
+      <c r="J17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>561</v>
+      </c>
+      <c r="B18" t="s">
+        <v>494</v>
+      </c>
+      <c r="C18" t="s">
+        <v>562</v>
+      </c>
+      <c r="D18" t="s">
+        <v>348</v>
+      </c>
+      <c r="E18" t="s">
+        <v>563</v>
+      </c>
+      <c r="F18" t="s">
+        <v>410</v>
+      </c>
+      <c r="G18" t="s">
+        <v>564</v>
+      </c>
+      <c r="H18" t="s">
+        <v>498</v>
+      </c>
+      <c r="I18" t="s">
+        <v>39</v>
+      </c>
+      <c r="J18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>565</v>
+      </c>
+      <c r="B19" t="s">
+        <v>494</v>
+      </c>
+      <c r="C19" t="s">
+        <v>566</v>
+      </c>
+      <c r="D19" t="s">
+        <v>348</v>
+      </c>
+      <c r="E19" t="s">
+        <v>567</v>
+      </c>
+      <c r="F19" t="s">
+        <v>410</v>
+      </c>
+      <c r="G19" t="s">
+        <v>568</v>
+      </c>
+      <c r="H19" t="s">
+        <v>498</v>
+      </c>
+      <c r="I19" t="s">
+        <v>39</v>
+      </c>
+      <c r="J19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>569</v>
+      </c>
+      <c r="B20" t="s">
+        <v>494</v>
+      </c>
+      <c r="C20" t="s">
+        <v>570</v>
+      </c>
+      <c r="D20" t="s">
+        <v>348</v>
+      </c>
+      <c r="E20" t="s">
+        <v>571</v>
+      </c>
+      <c r="F20" t="s">
+        <v>410</v>
+      </c>
+      <c r="G20" t="s">
+        <v>572</v>
+      </c>
+      <c r="H20" t="s">
+        <v>498</v>
+      </c>
+      <c r="I20" t="s">
+        <v>39</v>
+      </c>
+      <c r="J20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>573</v>
+      </c>
+      <c r="B21" t="s">
+        <v>494</v>
+      </c>
+      <c r="C21" t="s">
+        <v>574</v>
+      </c>
+      <c r="D21" t="s">
+        <v>575</v>
+      </c>
+      <c r="E21" t="s">
+        <v>576</v>
+      </c>
+      <c r="F21" t="s">
+        <v>410</v>
+      </c>
+      <c r="G21" t="s">
+        <v>577</v>
+      </c>
+      <c r="H21" t="s">
+        <v>498</v>
+      </c>
+      <c r="I21" t="s">
+        <v>39</v>
+      </c>
+      <c r="J21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>578</v>
+      </c>
+      <c r="B22" t="s">
+        <v>494</v>
+      </c>
+      <c r="C22" t="s">
+        <v>579</v>
+      </c>
+      <c r="D22" t="s">
+        <v>580</v>
+      </c>
+      <c r="E22" t="s">
+        <v>581</v>
+      </c>
+      <c r="F22" t="s">
+        <v>410</v>
+      </c>
+      <c r="G22" t="s">
+        <v>582</v>
+      </c>
+      <c r="H22" t="s">
+        <v>498</v>
+      </c>
+      <c r="I22" t="s">
+        <v>39</v>
+      </c>
+      <c r="J22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>583</v>
+      </c>
+      <c r="B23" t="s">
+        <v>494</v>
+      </c>
+      <c r="C23" t="s">
+        <v>584</v>
+      </c>
+      <c r="D23" t="s">
+        <v>348</v>
+      </c>
+      <c r="E23" t="s">
+        <v>585</v>
+      </c>
+      <c r="F23" t="s">
+        <v>410</v>
+      </c>
+      <c r="G23" t="s">
+        <v>586</v>
+      </c>
+      <c r="H23" t="s">
+        <v>498</v>
+      </c>
+      <c r="I23" t="s">
+        <v>39</v>
+      </c>
+      <c r="J23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>587</v>
+      </c>
+      <c r="B24" t="s">
+        <v>494</v>
+      </c>
+      <c r="C24" t="s">
+        <v>588</v>
+      </c>
+      <c r="D24" t="s">
+        <v>580</v>
+      </c>
+      <c r="E24" t="s">
+        <v>589</v>
+      </c>
+      <c r="F24" t="s">
+        <v>410</v>
+      </c>
+      <c r="G24" t="s">
+        <v>590</v>
+      </c>
+      <c r="H24" t="s">
+        <v>498</v>
+      </c>
+      <c r="I24" t="s">
+        <v>39</v>
+      </c>
+      <c r="J24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>591</v>
+      </c>
+      <c r="B25" t="s">
+        <v>494</v>
+      </c>
+      <c r="C25" t="s">
+        <v>592</v>
+      </c>
+      <c r="D25" t="s">
+        <v>593</v>
+      </c>
+      <c r="E25" t="s">
+        <v>594</v>
+      </c>
+      <c r="F25" t="s">
+        <v>410</v>
+      </c>
+      <c r="G25" t="s">
+        <v>595</v>
+      </c>
+      <c r="H25" t="s">
+        <v>498</v>
+      </c>
+      <c r="I25" t="s">
+        <v>39</v>
+      </c>
+      <c r="J25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>596</v>
+      </c>
+      <c r="B26" t="s">
+        <v>494</v>
+      </c>
+      <c r="C26" t="s">
+        <v>597</v>
+      </c>
+      <c r="D26" t="s">
+        <v>593</v>
+      </c>
+      <c r="E26" t="s">
+        <v>598</v>
+      </c>
+      <c r="F26" t="s">
+        <v>410</v>
+      </c>
+      <c r="G26" t="s">
+        <v>599</v>
+      </c>
+      <c r="H26" t="s">
+        <v>498</v>
+      </c>
+      <c r="I26" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>600</v>
+      </c>
+      <c r="B27" t="s">
+        <v>494</v>
+      </c>
+      <c r="C27" t="s">
+        <v>601</v>
+      </c>
+      <c r="D27" t="s">
+        <v>602</v>
+      </c>
+      <c r="E27" t="s">
+        <v>603</v>
+      </c>
+      <c r="F27" t="s">
+        <v>410</v>
+      </c>
+      <c r="G27" t="s">
+        <v>604</v>
+      </c>
+      <c r="H27" t="s">
+        <v>498</v>
+      </c>
+      <c r="I27" t="s">
+        <v>39</v>
+      </c>
+      <c r="J27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>605</v>
+      </c>
+      <c r="B28" t="s">
+        <v>494</v>
+      </c>
+      <c r="C28" t="s">
+        <v>606</v>
+      </c>
+      <c r="D28" t="s">
+        <v>602</v>
+      </c>
+      <c r="E28" t="s">
+        <v>607</v>
+      </c>
+      <c r="F28" t="s">
+        <v>410</v>
+      </c>
+      <c r="G28" t="s">
+        <v>604</v>
+      </c>
+      <c r="H28" t="s">
+        <v>498</v>
+      </c>
+      <c r="I28" t="s">
+        <v>39</v>
+      </c>
+      <c r="J28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>608</v>
+      </c>
+      <c r="B29" t="s">
+        <v>494</v>
+      </c>
+      <c r="C29" t="s">
+        <v>609</v>
+      </c>
+      <c r="D29" t="s">
+        <v>602</v>
+      </c>
+      <c r="E29" t="s">
+        <v>610</v>
+      </c>
+      <c r="F29" t="s">
+        <v>410</v>
+      </c>
+      <c r="G29" t="s">
+        <v>604</v>
+      </c>
+      <c r="H29" t="s">
+        <v>498</v>
+      </c>
+      <c r="I29" t="s">
+        <v>39</v>
+      </c>
+      <c r="J29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>611</v>
+      </c>
+      <c r="B30" t="s">
+        <v>494</v>
+      </c>
+      <c r="C30" t="s">
+        <v>612</v>
+      </c>
+      <c r="D30" t="s">
+        <v>602</v>
+      </c>
+      <c r="E30" t="s">
+        <v>613</v>
+      </c>
+      <c r="F30" t="s">
+        <v>410</v>
+      </c>
+      <c r="G30" t="s">
+        <v>604</v>
+      </c>
+      <c r="H30" t="s">
+        <v>498</v>
+      </c>
+      <c r="I30" t="s">
+        <v>39</v>
+      </c>
+      <c r="J30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>614</v>
+      </c>
+      <c r="B31" t="s">
+        <v>494</v>
+      </c>
+      <c r="C31" t="s">
+        <v>615</v>
+      </c>
+      <c r="D31" t="s">
+        <v>602</v>
+      </c>
+      <c r="E31" t="s">
+        <v>616</v>
+      </c>
+      <c r="F31" t="s">
+        <v>410</v>
+      </c>
+      <c r="G31" t="s">
+        <v>604</v>
+      </c>
+      <c r="H31" t="s">
+        <v>498</v>
+      </c>
+      <c r="I31" t="s">
+        <v>39</v>
+      </c>
+      <c r="J31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>617</v>
+      </c>
+      <c r="B32" t="s">
+        <v>494</v>
+      </c>
+      <c r="C32" t="s">
+        <v>618</v>
+      </c>
+      <c r="D32" t="s">
+        <v>602</v>
+      </c>
+      <c r="E32" t="s">
+        <v>619</v>
+      </c>
+      <c r="F32" t="s">
+        <v>410</v>
+      </c>
+      <c r="G32" t="s">
+        <v>604</v>
+      </c>
+      <c r="H32" t="s">
+        <v>498</v>
+      </c>
+      <c r="I32" t="s">
+        <v>39</v>
+      </c>
+      <c r="J32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>620</v>
+      </c>
+      <c r="B33" t="s">
+        <v>494</v>
+      </c>
+      <c r="C33" t="s">
+        <v>621</v>
+      </c>
+      <c r="D33" t="s">
+        <v>602</v>
+      </c>
+      <c r="E33" t="s">
+        <v>622</v>
+      </c>
+      <c r="F33" t="s">
+        <v>527</v>
+      </c>
+      <c r="G33" t="s">
+        <v>623</v>
+      </c>
+      <c r="H33" t="s">
+        <v>498</v>
+      </c>
+      <c r="I33" t="s">
+        <v>39</v>
+      </c>
+      <c r="J33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>624</v>
+      </c>
+      <c r="B34" t="s">
+        <v>494</v>
+      </c>
+      <c r="C34" t="s">
+        <v>625</v>
+      </c>
+      <c r="D34" t="s">
+        <v>602</v>
+      </c>
+      <c r="E34" t="s">
+        <v>626</v>
+      </c>
+      <c r="F34" t="s">
+        <v>527</v>
+      </c>
+      <c r="G34" t="s">
+        <v>627</v>
+      </c>
+      <c r="H34" t="s">
+        <v>498</v>
+      </c>
+      <c r="I34" t="s">
+        <v>39</v>
+      </c>
+      <c r="J34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>628</v>
+      </c>
+      <c r="B35" t="s">
+        <v>494</v>
+      </c>
+      <c r="C35" t="s">
+        <v>629</v>
+      </c>
+      <c r="D35" t="s">
+        <v>602</v>
+      </c>
+      <c r="E35" t="s">
+        <v>630</v>
+      </c>
+      <c r="F35" t="s">
+        <v>527</v>
+      </c>
+      <c r="G35" t="s">
+        <v>631</v>
+      </c>
+      <c r="H35" t="s">
+        <v>498</v>
+      </c>
+      <c r="I35" t="s">
+        <v>39</v>
+      </c>
+      <c r="J35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>632</v>
+      </c>
+      <c r="B36" t="s">
+        <v>494</v>
+      </c>
+      <c r="C36" t="s">
+        <v>633</v>
+      </c>
+      <c r="D36" t="s">
+        <v>602</v>
+      </c>
+      <c r="E36" t="s">
+        <v>634</v>
+      </c>
+      <c r="F36" t="s">
+        <v>527</v>
+      </c>
+      <c r="G36" t="s">
+        <v>635</v>
+      </c>
+      <c r="H36" t="s">
+        <v>498</v>
+      </c>
+      <c r="I36" t="s">
+        <v>39</v>
+      </c>
+      <c r="J36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>636</v>
+      </c>
+      <c r="B37" t="s">
+        <v>494</v>
+      </c>
+      <c r="C37" t="s">
+        <v>637</v>
+      </c>
+      <c r="D37" t="s">
+        <v>638</v>
+      </c>
+      <c r="E37" t="s">
+        <v>639</v>
+      </c>
+      <c r="F37" t="s">
+        <v>472</v>
+      </c>
+      <c r="G37" t="s">
+        <v>640</v>
+      </c>
+      <c r="H37" t="s">
+        <v>498</v>
+      </c>
+      <c r="I37" t="s">
+        <v>39</v>
+      </c>
+      <c r="J37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>641</v>
+      </c>
+      <c r="B38" t="s">
+        <v>494</v>
+      </c>
+      <c r="C38" t="s">
+        <v>642</v>
+      </c>
+      <c r="D38" t="s">
+        <v>638</v>
+      </c>
+      <c r="E38" t="s">
+        <v>643</v>
+      </c>
+      <c r="F38" t="s">
+        <v>472</v>
+      </c>
+      <c r="G38" t="s">
+        <v>644</v>
+      </c>
+      <c r="H38" t="s">
+        <v>498</v>
+      </c>
+      <c r="I38" t="s">
+        <v>39</v>
+      </c>
+      <c r="J38" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>645</v>
+      </c>
+      <c r="B39" t="s">
+        <v>494</v>
+      </c>
+      <c r="C39" t="s">
+        <v>646</v>
+      </c>
+      <c r="D39" t="s">
+        <v>638</v>
+      </c>
+      <c r="E39" t="s">
+        <v>643</v>
+      </c>
+      <c r="F39" t="s">
+        <v>472</v>
+      </c>
+      <c r="G39" t="s">
+        <v>647</v>
+      </c>
+      <c r="H39" t="s">
+        <v>498</v>
+      </c>
+      <c r="I39" t="s">
+        <v>39</v>
+      </c>
+      <c r="J39" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>